<commit_message>
updating my timesheet ~Harvey
</commit_message>
<xml_diff>
--- a/CONFIG/Timesheets/hac22.xlsx
+++ b/CONFIG/Timesheets/hac22.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1500" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Writing a brief overview of classes</t>
+  </si>
+  <si>
+    <t>Week:Nov20th-Nov27th</t>
+  </si>
+  <si>
+    <t>Prototpying JSON Generation</t>
+  </si>
+  <si>
+    <t>Documentation for the Design Spec</t>
   </si>
 </sst>
 </file>
@@ -125,8 +134,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -142,15 +163,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C27"/>
+  <dimension ref="A4:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -625,22 +658,65 @@
         <v>2.4305555555555556E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="B23" t="s">
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C22" s="1">
         <f>SUM(C19:C21)</f>
         <v>0.125</v>
       </c>
     </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
     <row r="27" spans="1:3">
       <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
+        <f>SUM(C25:C30)</f>
+        <v>1.1041666666666667</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="1">
-        <f>SUM(C9+C16+C23)</f>
-        <v>0.69791666666666663</v>
+      <c r="C34" s="1">
+        <f>SUM(C9+C16+C22+C31)</f>
+        <v>1.8020833333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating timesheet based on metting
</commit_message>
<xml_diff>
--- a/CONFIG/Timesheets/hac22.xlsx
+++ b/CONFIG/Timesheets/hac22.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,14 +512,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
@@ -697,8 +697,8 @@
       <c r="B27" t="s">
         <v>2</v>
       </c>
-      <c r="C27">
-        <v>1</v>
+      <c r="C27" s="1">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -707,7 +707,7 @@
       </c>
       <c r="C31" s="1">
         <f>SUM(C25:C30)</f>
-        <v>1.1041666666666667</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="34" spans="2:3">
@@ -716,7 +716,7 @@
       </c>
       <c r="C34" s="1">
         <f>SUM(C9+C16+C22+C31)</f>
-        <v>1.8020833333333335</v>
+        <v>0.88541666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating timesheet and Key Algorithms document
</commit_message>
<xml_diff>
--- a/CONFIG/Timesheets/hac22.xlsx
+++ b/CONFIG/Timesheets/hac22.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Documentation for the Design Spec</t>
+  </si>
+  <si>
+    <t>Looking into MIME/HTTP Post</t>
+  </si>
+  <si>
+    <t>Week:Nov27th-Dec3rd</t>
+  </si>
+  <si>
+    <t>Write up of algorithms</t>
+  </si>
+  <si>
+    <t>Research into algorithms</t>
   </si>
 </sst>
 </file>
@@ -513,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:C34"/>
+  <dimension ref="A4:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -701,22 +713,98 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1">
+        <f>SUM(C25:C28)</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="31" spans="1:3">
       <c r="B31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="1">
-        <f>SUM(C25:C30)</f>
+      <c r="C35" s="1">
+        <f>SUM(C32:C34)</f>
         <v>0.22916666666666669</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="B34" t="s">
+    <row r="36" spans="2:4">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="1">
-        <f>SUM(C9+C16+C22+C31)</f>
-        <v>0.92708333333333326</v>
+      <c r="C44" s="1">
+        <f>SUM(C9,C16,C22,C29,C35)</f>
+        <v>1.21875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>